<commit_message>
Got ANOVA results for enzyme parameters for 6 enzymes
The enzymes I got ANOVA results for so far are AG, AP, BG, BX, CBH, and LAP. Enzymes I have left are NAG and PPO
</commit_message>
<xml_diff>
--- a/Statistical analyses/ANOVA results.xlsx
+++ b/Statistical analyses/ANOVA results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Statistical analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1E6B7B-D0A4-4873-845E-9E6388BB5C6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBB8DD6-5E23-4F6A-A899-583446E3D600}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="20">
   <si>
     <t>Enzyme</t>
   </si>
@@ -415,7 +415,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,20 +511,104 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -548,7 +632,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,7 +709,7 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -644,20 +728,104 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Got ANOVA results for all enzyme parameters, yay
Aight so now, Tukey posthoc. I'm probably gonna visualize Tukey posthoc results with boxplots.
</commit_message>
<xml_diff>
--- a/Statistical analyses/ANOVA results.xlsx
+++ b/Statistical analyses/ANOVA results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Statistical analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBB8DD6-5E23-4F6A-A899-583446E3D600}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127DFCCF-146C-401F-A4CE-81A064FEF9D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="23">
   <si>
     <t>Enzyme</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>***</t>
+  </si>
+  <si>
+    <t>red = all interactions are non-significant</t>
+  </si>
+  <si>
+    <t>green = non-significant interactions, significant main effects</t>
+  </si>
+  <si>
+    <t>yellow = non-significant interations, non-significant main effects</t>
   </si>
 </sst>
 </file>
@@ -109,12 +118,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,9 +156,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +442,278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014A953-EC86-410A-AF55-A076AABF3B1D}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,28 +754,28 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -486,76 +784,76 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -570,7 +868,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
@@ -586,28 +884,28 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -615,227 +913,52 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014A953-EC86-410A-AF55-A076AABF3B1D}">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>15</v>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Annotating Tukey posthoc results
I used the Tukey posthoc results Excel files to make groups by significant interactions or main effects, and recorded these groups on Excel files with "annotated" in their names. These files will then be used to annotate boxplots, which I will make in the next couple of days.

Most of the deleted files are files in which ANOVA results indicate significant interactions or main effects but Tukey posthoc results indicate otherwise, indicating that I committed Type 1 errors with their ANOVA results. Good thing the Tukey is here to catch this Type 1 error. I also deleted the MANOVA excel results file and instead copied the MANOVA results into the ANOVA results file.
</commit_message>
<xml_diff>
--- a/Statistical analyses/ANOVA results.xlsx
+++ b/Statistical analyses/ANOVA results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Statistical analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127DFCCF-146C-401F-A4CE-81A064FEF9D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60074B69-4FDF-411D-AE33-5F2566BAB0A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="24">
   <si>
     <t>Enzyme</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>yellow = non-significant interations, non-significant main effects</t>
+  </si>
+  <si>
+    <t>MANOVA</t>
   </si>
 </sst>
 </file>
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,6 +705,32 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -710,10 +739,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014A953-EC86-410A-AF55-A076AABF3B1D}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,6 +990,32 @@
         <v>16</v>
       </c>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Litter chemistry ANOVAs and effect sizes for litter chemistry and Vmax
I calculated partial eta-squared and classical eta-squared as measures of ANOVA effect sizes, though I only recorded partial eta-squared values. I then conducted ANOVAs on the litter chemistry functional groups, as well as calculated eta-squared for them.

Something of note is that, although precipitation hardly influences enzyme activity, it does have a medium-large effect on litter chemistry. This suggests that precipitation influences enzyme kinetics itself.
</commit_message>
<xml_diff>
--- a/Statistical analyses/ANOVA results.xlsx
+++ b/Statistical analyses/ANOVA results.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Statistical analyses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial-enzyme-activity-in-leaf-litter\Statistical analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60074B69-4FDF-411D-AE33-5F2566BAB0A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C81B1D-CF2D-45E9-B313-A2A930B9FE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
     <sheet name="Km" sheetId="3" r:id="rId2"/>
+    <sheet name="litterChemistry" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="31">
   <si>
     <t>Enzyme</t>
   </si>
@@ -98,6 +99,27 @@
   </si>
   <si>
     <t>MANOVA</t>
+  </si>
+  <si>
+    <t>functionalGroup</t>
+  </si>
+  <si>
+    <t>glycosidicBond</t>
+  </si>
+  <si>
+    <t>C_O_stretching</t>
+  </si>
+  <si>
+    <t>carboEster</t>
+  </si>
+  <si>
+    <t>lipid</t>
+  </si>
+  <si>
+    <t>alkane</t>
+  </si>
+  <si>
+    <t>amide</t>
   </si>
 </sst>
 </file>
@@ -448,7 +470,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014A953-EC86-410A-AF55-A076AABF3B1D}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1020,4 +1042,211 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D258B1-11EA-499A-8DC2-5CAE40970808}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Re-analyzed carbohydrate esters & amides
Ashish originally had 2 categories for carbohydrate esters and 2 categories for amides, each of which occupies a specific FTIR spectral range. I combined these 2 categories of each compound into 1 category so that there's only spectral area for carbohydrate esters and spectral area amides rather than spectral area for 2 categories of carbohydrate esters and spectral area for 2 categories of amides.

Ashish told me that combining spectral area like that is a bad idea. So, I re-analyzed these 2 functional groups in their original categories using factorial ANOVAs and Tukey's, and created boxplots for them.
</commit_message>
<xml_diff>
--- a/Statistical analyses/ANOVA results.xlsx
+++ b/Statistical analyses/ANOVA results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial-enzyme-activity-in-leaf-litter\Statistical analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C81B1D-CF2D-45E9-B313-A2A930B9FE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8761C3D0-BE02-4835-BF16-11B73F7CCA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="35">
   <si>
     <t>Enzyme</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>amide</t>
+  </si>
+  <si>
+    <t>carboEster1</t>
+  </si>
+  <si>
+    <t>carboEster2</t>
+  </si>
+  <si>
+    <t>amide1</t>
+  </si>
+  <si>
+    <t>amide2</t>
   </si>
 </sst>
 </file>
@@ -169,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -177,16 +189,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D258B1-11EA-499A-8DC2-5CAE40970808}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,184 +1094,288 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Shapiro-Wilk and ANOVA on CAZyme domains
So I checked the CAZyme data for normality using the Shapiro-Wilk test. While some treatments weren't normal, Conducting a Box-Cox did not remove this lack of normality. In addition, the dataset, overall, appears fairly normal. So, whatever, I just conducted ANOVAs on them, and I'm going to follow up with Tukey's later.
</commit_message>
<xml_diff>
--- a/Statistical analyses/ANOVA results.xlsx
+++ b/Statistical analyses/ANOVA results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial-enzyme-activity-in-leaf-litter\Statistical analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8761C3D0-BE02-4835-BF16-11B73F7CCA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3D2FE8-AB17-4F98-83E6-A5F8C23FCC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
     <sheet name="Km" sheetId="3" r:id="rId2"/>
     <sheet name="litterChemistry" sheetId="4" r:id="rId3"/>
+    <sheet name="CAZyme domains" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="50">
   <si>
     <t>Enzyme</t>
   </si>
@@ -132,6 +133,51 @@
   </si>
   <si>
     <t>amide2</t>
+  </si>
+  <si>
+    <t>Hemicellulose</t>
+  </si>
+  <si>
+    <t>Lignin</t>
+  </si>
+  <si>
+    <t>Polysaccharide</t>
+  </si>
+  <si>
+    <t>Oligosaccharides</t>
+  </si>
+  <si>
+    <t>Cell_wall</t>
+  </si>
+  <si>
+    <t>Inulin</t>
+  </si>
+  <si>
+    <t>Starch</t>
+  </si>
+  <si>
+    <t>Trehalose</t>
+  </si>
+  <si>
+    <t>Cellulose</t>
+  </si>
+  <si>
+    <t>Pectin</t>
+  </si>
+  <si>
+    <t>Glycogen</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Peptidoglycan</t>
+  </si>
+  <si>
+    <t>Chitin</t>
+  </si>
+  <si>
+    <t>Substrate</t>
   </si>
 </sst>
 </file>
@@ -1077,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D258B1-11EA-499A-8DC2-5CAE40970808}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1382,4 +1428,419 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E360F3A-AF75-445A-A5DE-54298D2C4BC4}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>